<commit_message>
add new project for dolby
</commit_message>
<xml_diff>
--- a/performance_log_group/performane.xlsx
+++ b/performance_log_group/performane.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -59,24 +59,6 @@
   </si>
   <si>
     <t>max_bits</t>
-  </si>
-  <si>
-    <t>UHD_VOD_COUNT_DOWN_GIRL_GIRL_GIRL_2ND_02.ES</t>
-  </si>
-  <si>
-    <t>NEPAL_ADVENTURES_OF_TEAMSUPERTRAMP.IVF</t>
-  </si>
-  <si>
-    <t>NETFLIX_HEVCM10PL51-6000FPS-16000KBPS-3840X2160-1014520_5033638636_CUT500M.265</t>
-  </si>
-  <si>
-    <t>STREET1_1_4096X2176_FR60_BD10_GF_DIST_10_L51.WEBM.IVF</t>
-  </si>
-  <si>
-    <t>STREET1_1_4096X2176_FR60_BD8_GF_DIST_10_L51.WEBM.IVF</t>
-  </si>
-  <si>
-    <t>TRANSFORMERS_4_2014_4K_OFFICIAL_TRAILER_-_60FPS_SVP-HFR_2160P.IVF</t>
   </si>
 </sst>
 </file>
@@ -408,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:P10"/>
+  <dimension ref="A3:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,314 +443,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>6003</v>
-      </c>
-      <c r="E4">
-        <v>6003</v>
-      </c>
-      <c r="F4">
-        <v>60</v>
-      </c>
-      <c r="G4">
-        <v>3840</v>
-      </c>
-      <c r="H4">
-        <v>2176</v>
-      </c>
-      <c r="I4">
-        <v>32640</v>
-      </c>
-      <c r="J4">
-        <v>15822261</v>
-      </c>
-      <c r="K4">
-        <v>8922670</v>
-      </c>
-      <c r="L4">
-        <v>4823009</v>
-      </c>
-      <c r="M4">
-        <v>77683</v>
-      </c>
-      <c r="N4">
-        <v>7878555</v>
-      </c>
-      <c r="O4">
-        <v>505434</v>
-      </c>
-      <c r="P4">
-        <v>5634738</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>3901</v>
-      </c>
-      <c r="E5">
-        <v>3491</v>
-      </c>
-      <c r="F5">
-        <v>60</v>
-      </c>
-      <c r="G5">
-        <v>3856</v>
-      </c>
-      <c r="H5">
-        <v>2176</v>
-      </c>
-      <c r="I5">
-        <v>32640</v>
-      </c>
-      <c r="J5">
-        <v>12548077</v>
-      </c>
-      <c r="K5">
-        <v>7641435</v>
-      </c>
-      <c r="L5">
-        <v>6140853</v>
-      </c>
-      <c r="M5">
-        <v>907107</v>
-      </c>
-      <c r="N5">
-        <v>11928724</v>
-      </c>
-      <c r="O5">
-        <v>694416</v>
-      </c>
-      <c r="P5">
-        <v>6792713</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>6002</v>
-      </c>
-      <c r="E6">
-        <v>6002</v>
-      </c>
-      <c r="F6">
-        <v>60</v>
-      </c>
-      <c r="G6">
-        <v>3840</v>
-      </c>
-      <c r="H6">
-        <v>2176</v>
-      </c>
-      <c r="I6">
-        <v>32640</v>
-      </c>
-      <c r="J6">
-        <v>16106040</v>
-      </c>
-      <c r="K6">
-        <v>8912545</v>
-      </c>
-      <c r="L6">
-        <v>5196444</v>
-      </c>
-      <c r="M6">
-        <v>211809</v>
-      </c>
-      <c r="N6">
-        <v>7614191</v>
-      </c>
-      <c r="O6">
-        <v>268844</v>
-      </c>
-      <c r="P6">
-        <v>6103116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>660</v>
-      </c>
-      <c r="E7">
-        <v>600</v>
-      </c>
-      <c r="F7">
-        <v>60</v>
-      </c>
-      <c r="G7">
-        <v>4112</v>
-      </c>
-      <c r="H7">
-        <v>2176</v>
-      </c>
-      <c r="I7">
-        <v>34816</v>
-      </c>
-      <c r="J7">
-        <v>24195978</v>
-      </c>
-      <c r="K7">
-        <v>12235025</v>
-      </c>
-      <c r="L7">
-        <v>9578116</v>
-      </c>
-      <c r="M7">
-        <v>1423425</v>
-      </c>
-      <c r="N7">
-        <v>19691629</v>
-      </c>
-      <c r="O7">
-        <v>1787870</v>
-      </c>
-      <c r="P7">
-        <v>17193105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8">
-        <v>660</v>
-      </c>
-      <c r="E8">
-        <v>600</v>
-      </c>
-      <c r="F8">
-        <v>60</v>
-      </c>
-      <c r="G8">
-        <v>4112</v>
-      </c>
-      <c r="H8">
-        <v>2176</v>
-      </c>
-      <c r="I8">
-        <v>34816</v>
-      </c>
-      <c r="J8">
-        <v>17542659</v>
-      </c>
-      <c r="K8">
-        <v>7477356</v>
-      </c>
-      <c r="L8">
-        <v>12436009</v>
-      </c>
-      <c r="M8">
-        <v>1411563</v>
-      </c>
-      <c r="N8">
-        <v>23896751</v>
-      </c>
-      <c r="O8">
-        <v>1785813</v>
-      </c>
-      <c r="P8">
-        <v>15930286</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>4630</v>
-      </c>
-      <c r="E9">
-        <v>4444</v>
-      </c>
-      <c r="F9">
-        <v>60</v>
-      </c>
-      <c r="G9">
-        <v>3856</v>
-      </c>
-      <c r="H9">
-        <v>2176</v>
-      </c>
-      <c r="I9">
-        <v>32640</v>
-      </c>
-      <c r="J9">
-        <v>5992949</v>
-      </c>
-      <c r="K9">
-        <v>5548359</v>
-      </c>
-      <c r="L9">
-        <v>4773750</v>
-      </c>
-      <c r="M9">
-        <v>687385</v>
-      </c>
-      <c r="N9">
-        <v>7481905</v>
-      </c>
-      <c r="O9">
-        <v>292458</v>
-      </c>
-      <c r="P9">
-        <v>4920802</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>6003</v>
-      </c>
-      <c r="E10">
-        <v>6003</v>
-      </c>
-      <c r="F10">
-        <v>60</v>
-      </c>
-      <c r="G10">
-        <v>3840</v>
-      </c>
-      <c r="H10">
-        <v>2176</v>
-      </c>
-      <c r="I10">
-        <v>32640</v>
-      </c>
-      <c r="J10">
-        <v>15822261</v>
-      </c>
-      <c r="K10">
-        <v>8922670</v>
-      </c>
-      <c r="L10">
-        <v>4823009</v>
-      </c>
-      <c r="M10">
-        <v>77683</v>
-      </c>
-      <c r="N10">
-        <v>7878555</v>
-      </c>
-      <c r="O10">
-        <v>505434</v>
-      </c>
-      <c r="P10">
-        <v>5634738</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>